<commit_message>
update booking and saleOrder
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E9"/>
+  <dimension ref="B4:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -470,6 +470,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>445328338</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>